<commit_message>
fixes some part of the admin
</commit_message>
<xml_diff>
--- a/source_kenn/debug/cjobs.xlsx
+++ b/source_kenn/debug/cjobs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -196,6 +196,43 @@
   </si>
   <si>
     <t>to examine here -- app_cache_functions.php</t>
+  </si>
+  <si>
+    <t>//Check IPFW -- index.php</t>
+  </si>
+  <si>
+    <t>html\cjobs10.htm</t>
+  </si>
+  <si>
+    <t>html\cjobs11.htm</t>
+  </si>
+  <si>
+    <t>Index_functions.php -- $_SESSION  -- [sess_visitor] =&gt; Array
+        (
+            [ip] =&gt; ::1
+            [stat_vi] =&gt; 5
+        )</t>
+  </si>
+  <si>
+    <t>html\cjobs12.htm</t>
+  </si>
+  <si>
+    <t>app_cache_functions.php -- $cache_params_array</t>
+  </si>
+  <si>
+    <t>html\cjobs13.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app_cache_functions.php -- write_mydata_cache - Undefined variable: fname </t>
+  </si>
+  <si>
+    <t>html\cjobs14.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app_cache_functions.php -- write_mydata_cache - Undefined variable: cache_dir_innerpath </t>
+  </si>
+  <si>
+    <t>app_cache_functions.php -- $cache_data_filename = C:\wamp\www\cjobs\management/cache/smarty_frontend/0/search_result/ipfirewall/3a524c7664d88bb904dd01e94f54326d</t>
   </si>
 </sst>
 </file>
@@ -273,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -283,6 +320,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -589,13 +632,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,6 +921,68 @@
       </c>
       <c r="E24" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>41395</v>
+      </c>
+      <c r="C25" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>41395</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>41395</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>41395</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -895,9 +1000,14 @@
     <hyperlink ref="C13" r:id="rId11"/>
     <hyperlink ref="C19" r:id="rId12"/>
     <hyperlink ref="B23" r:id="rId13"/>
+    <hyperlink ref="C26" r:id="rId14"/>
+    <hyperlink ref="C27" r:id="rId15"/>
+    <hyperlink ref="C28" r:id="rId16"/>
+    <hyperlink ref="C29" r:id="rId17"/>
+    <hyperlink ref="C30" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId14"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>